<commit_message>
chore: fix format test
</commit_message>
<xml_diff>
--- a/test/expected/format.xlsx
+++ b/test/expected/format.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>bold</t>
   </si>
   <si>
     <t>italic</t>
+  </si>
+  <si>
+    <t>rot45</t>
+  </si>
+  <si>
+    <t>strikethrough</t>
   </si>
   <si>
     <t>underline single</t>
@@ -44,8 +50,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/m/d h:mm"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -129,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -148,6 +155,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,13 +450,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,33 +469,45 @@
       <c r="D1" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1" s="11">
-        <v>36903</v>
-      </c>
-      <c r="F1" s="11">
-        <v>47756.99998842592</v>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I1" s="7">
         <f>PI()</f>
         <v>0</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="N1" s="11">
+        <v>36903</v>
+      </c>
+      <c r="O1" s="11">
+        <v>47756.99998842592</v>
+      </c>
+      <c r="P1" s="12">
+        <v>36903</v>
+      </c>
+      <c r="Q1" s="12">
+        <v>47756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add worksheet.writeDateWithFormat and ExcelDateTime (#115)
* feat: add ExcelDateTime

* feat: add writeDateWithFormat to worksheet

* chore: fix format test

* chore: add xlsx::IntoExcelDateTime for ExcelDateTime & refactor

* chore: revert write datetime

* feat: accept Date object & ExcelDateTime

* chore: add datetime test
</commit_message>
<xml_diff>
--- a/test/expected/format.xlsx
+++ b/test/expected/format.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>bold</t>
   </si>
   <si>
     <t>italic</t>
+  </si>
+  <si>
+    <t>rot45</t>
+  </si>
+  <si>
+    <t>strikethrough</t>
   </si>
   <si>
     <t>underline single</t>
@@ -44,8 +50,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy/m/d h:mm"/>
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -129,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -148,6 +155,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,13 +450,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,33 +469,45 @@
       <c r="D1" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="E1" s="11">
-        <v>36903</v>
-      </c>
-      <c r="F1" s="11">
-        <v>47756.99998842592</v>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I1" s="7">
         <f>PI()</f>
         <v>0</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="N1" s="11">
+        <v>36903</v>
+      </c>
+      <c r="O1" s="11">
+        <v>47756.99998842592</v>
+      </c>
+      <c r="P1" s="12">
+        <v>36903</v>
+      </c>
+      <c r="Q1" s="12">
+        <v>47756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>